<commit_message>
v0.11: Add arrow square red and green.
</commit_message>
<xml_diff>
--- a/rsc/all_squares.xlsx
+++ b/rsc/all_squares.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t xml:space="preserve">Start</t>
   </si>
@@ -90,6 +90,18 @@
   </si>
   <si>
     <t xml:space="preserve">VNL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRVU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRVR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRVD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRVL</t>
   </si>
   <si>
     <t xml:space="preserve">bg</t>
@@ -102,7 +114,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -131,6 +143,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -218,7 +235,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -260,6 +277,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -340,10 +361,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:E8"/>
+  <dimension ref="B2:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.9296875" defaultRowHeight="39.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -433,6 +454,20 @@
       </c>
       <c r="E8" s="1" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -464,24 +499,24 @@
   <sheetData>
     <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
v0.12: Add ice square background.
</commit_message>
<xml_diff>
--- a/rsc/all_squares.xlsx
+++ b/rsc/all_squares.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="maze" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t xml:space="preserve">Start</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t xml:space="preserve">bg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ice</t>
   </si>
 </sst>
 </file>
@@ -114,7 +117,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -143,11 +146,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -280,7 +278,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -363,7 +361,7 @@
   </sheetPr>
   <dimension ref="B2:E9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -488,8 +486,8 @@
   </sheetPr>
   <dimension ref="B2:D8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.9296875" defaultRowHeight="39.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -500,6 +498,9 @@
     <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>